<commit_message>
added VAS, NDQ in list
</commit_message>
<xml_diff>
--- a/sip_calculator/input/ETF_list.xlsx
+++ b/sip_calculator/input/ETF_list.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="62">
   <si>
     <t>Country</t>
   </si>
@@ -193,6 +193,15 @@
   </si>
   <si>
     <t xml:space="preserve"> tracks S&amp;P/ASX 200.</t>
+  </si>
+  <si>
+    <t>VAS.AX</t>
+  </si>
+  <si>
+    <t>IVV.AX</t>
+  </si>
+  <si>
+    <t>NDQ.AX</t>
   </si>
 </sst>
 </file>
@@ -525,10 +534,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16:XFD27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -892,6 +901,39 @@
       </c>
       <c r="H15" t="s">
         <v>58</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" t="s">
+        <v>53</v>
+      </c>
+      <c r="B16" t="s">
+        <v>38</v>
+      </c>
+      <c r="C16" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" t="s">
+        <v>53</v>
+      </c>
+      <c r="B17" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" t="s">
+        <v>53</v>
+      </c>
+      <c r="B18" t="s">
+        <v>38</v>
+      </c>
+      <c r="C18" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>